<commit_message>
Paper and code updates
</commit_message>
<xml_diff>
--- a/Code/Liq_decile_stats.xlsx
+++ b/Code/Liq_decile_stats.xlsx
@@ -1,30 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5604ff08deb8de49/Documents/Research/Denmark/IncomeUncertaintyGit/Code/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_9D9B6563ACA446B510A9ABBCFF47716D4AAEA450" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{13BB610C-69F6-40FC-A425-A71B07D10836}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="22980" windowHeight="9276"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats - deciles for liquid asse" sheetId="1" r:id="rId1"/>
-    <sheet name="Stats - medians" sheetId="3" r:id="rId2"/>
-    <sheet name="Quantile dynamics" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="Stats - medians" sheetId="3" r:id="rId3"/>
+    <sheet name="Quantile dynamics" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="descriptives_SCF" localSheetId="0">'Stats - deciles for liquid asse'!$B$18:$L$28</definedName>
-    <definedName name="descriptives_SCF" localSheetId="1">'Stats - medians'!$B$18:$L$28</definedName>
+    <definedName name="descriptives_SCF" localSheetId="2">'Stats - medians'!$B$18:$L$28</definedName>
     <definedName name="liquid_decile_stats_ext_val" localSheetId="0">'Stats - deciles for liquid asse'!$B$3:$N$12</definedName>
-    <definedName name="liquid_decile_stats_ext_val" localSheetId="1">'Stats - medians'!$B$3:$M$12</definedName>
-    <definedName name="quantile_dynamics" localSheetId="2">'Quantile dynamics'!$U$1:$AA$57</definedName>
+    <definedName name="liquid_decile_stats_ext_val" localSheetId="2">'Stats - medians'!$B$3:$M$12</definedName>
+    <definedName name="quantile_dynamics" localSheetId="3">'Quantile dynamics'!$U$1:$AA$57</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="descriptives_SCF" type="6" refreshedVersion="4" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="descriptives_SCF" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="850" sourceFile="\\srv9dnbfil002\userhome\aku\Desktop\Cons hetero AEJ macro\descriptives_SCF.csv" comma="1">
       <textFields count="11">
         <textField/>
@@ -41,7 +59,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="descriptives_SCF1" type="6" refreshedVersion="4" background="1" saveData="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="descriptives_SCF1" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="850" sourceFile="\\srv9dnbfil002\userhome\aku\Desktop\Cons hetero AEJ macro\descriptives_SCF_medians.csv" comma="1">
       <textFields count="11">
         <textField/>
@@ -58,7 +76,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="liquid_decile_stats_ext_val" type="6" refreshedVersion="4" background="1" saveData="1">
+  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="liquid_decile_stats_ext_val" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="850" sourceFile="\\srv9dnbfil002\userhome\aku\Desktop\Cons hetero AEJ macro\liquid_decile_stats_ext_val.txt" comma="1">
       <textFields count="13">
         <textField/>
@@ -77,7 +95,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="liquid_decile_stats_ext_val1" type="6" refreshedVersion="4" background="1" saveData="1">
+  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="liquid_decile_stats_ext_val1" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="850" sourceFile="\\srv9dnbfil002\userhome\aku\Desktop\Cons hetero AEJ macro\liquid_decile_stats_ext_val_medians.txt" comma="1">
       <textFields count="13">
         <textField/>
@@ -96,7 +114,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="quantile_dynamics" type="6" refreshedVersion="4" background="1" saveData="1">
+  <connection id="5" xr16:uid="{00000000-0015-0000-FFFF-FFFF04000000}" name="quantile_dynamics" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="850" sourceFile="\\srv9dnbfil002\userhome\aku\Desktop\Cons hetero AEJ macro\quantile_dynamics.txt" space="1" consecutive="1">
       <textFields count="7">
         <textField/>
@@ -313,7 +331,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -381,10 +399,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -396,34 +414,1041 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stats - deciles for liquid asse'!$R$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>US</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Stats - deciles for liquid asse'!$R$4:$R$13</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>35.327247999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>325.25767000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>804.74680000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1532.9455</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2847.4751000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4884.2466000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8221.4992999999995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14750.228999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>31711.285</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>230122.02</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5E72-4C6C-B2E1-2D01323E0027}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stats - deciles for liquid asse'!$S$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DK</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Stats - deciles for liquid asse'!$S$4:$S$13</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>145.74630276564775</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1106.2218486171762</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2095.1072780203785</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3384.3058224163028</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5308.8056768558954</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8307.2931586608447</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13210.40422125182</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21870.841339155748</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39848.799126637554</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>138036.8806404658</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5E72-4C6C-B2E1-2D01323E0027}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="360462256"/>
+        <c:axId val="360458928"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="360462256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="360458928"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="360458928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="360462256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>198120</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BB1F837-769E-4920-8930-BF4BB5513BF0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="descriptives_SCF" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="descriptives_SCF" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="liquid_decile_stats_ext_val" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="liquid_decile_stats_ext_val" connectionId="3" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="liquid_decile_stats_ext_val" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="liquid_decile_stats_ext_val" connectionId="4" xr16:uid="{00000000-0016-0000-0100-000003000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="descriptives_SCF" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="descriptives_SCF" connectionId="2" xr16:uid="{00000000-0016-0000-0100-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="quantile_dynamics" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="quantile_dynamics" connectionId="5" xr16:uid="{00000000-0016-0000-0200-000004000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kontortema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kontor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -461,9 +1486,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kontor">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -496,9 +1521,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -531,9 +1573,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kontor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -706,11 +1765,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:AK13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -793,54 +1852,54 @@
       <c r="N2" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="9" t="str">
+      <c r="R2" s="8" t="str">
         <f>B2</f>
         <v>Liquid assets</v>
       </c>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9" t="str">
+      <c r="S2" s="8"/>
+      <c r="T2" s="8" t="str">
         <f>C2</f>
         <v>Net wealth</v>
       </c>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9" t="s">
+      <c r="U2" s="8"/>
+      <c r="V2" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9" t="s">
+      <c r="W2" s="8"/>
+      <c r="X2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9" t="str">
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8" t="str">
         <f>H2</f>
         <v>Age</v>
       </c>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9" t="str">
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8" t="str">
         <f>I2</f>
         <v>Homeowner</v>
       </c>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="9" t="str">
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8" t="str">
         <f>J2</f>
         <v>Carowner</v>
       </c>
-      <c r="AE2" s="9"/>
-      <c r="AF2" s="9" t="str">
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8" t="str">
         <f>K2</f>
         <v>URE</v>
       </c>
-      <c r="AG2" s="9"/>
-      <c r="AH2" s="9" t="str">
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="8" t="str">
         <f>L2</f>
         <v>NNP</v>
       </c>
-      <c r="AI2" s="9"/>
-      <c r="AJ2" s="9" t="str">
+      <c r="AI2" s="8"/>
+      <c r="AJ2" s="8" t="str">
         <f>M2</f>
         <v>Liabilities</v>
       </c>
-      <c r="AK2" s="9"/>
+      <c r="AK2" s="8"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -2188,18 +3247,18 @@
       </c>
     </row>
     <row r="14" spans="1:37" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="T14" s="8" t="s">
+      <c r="T14" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="U14" s="8"/>
-      <c r="V14" s="8" t="s">
+      <c r="U14" s="9"/>
+      <c r="V14" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="W14" s="8"/>
-      <c r="X14" s="8" t="s">
+      <c r="W14" s="9"/>
+      <c r="X14" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="Y14" s="8"/>
+      <c r="Y14" s="9"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -2623,6 +3682,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="T14:U14"/>
+    <mergeCell ref="X14:Y14"/>
+    <mergeCell ref="V14:W14"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
     <mergeCell ref="AH2:AI2"/>
     <mergeCell ref="AJ2:AK2"/>
     <mergeCell ref="R2:S2"/>
@@ -2631,19 +3695,27 @@
     <mergeCell ref="X2:Y2"/>
     <mergeCell ref="Z2:AA2"/>
     <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="T14:U14"/>
-    <mergeCell ref="X14:Y14"/>
-    <mergeCell ref="V14:W14"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19C06DED-5DAC-4349-B42A-3816447C7742}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK28"/>
   <sheetViews>
     <sheetView topLeftCell="R1" workbookViewId="0">
@@ -2732,54 +3804,54 @@
       <c r="M2" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="9" t="str">
+      <c r="R2" s="8" t="str">
         <f>B2</f>
         <v>Liquid assets</v>
       </c>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9" t="str">
+      <c r="S2" s="8"/>
+      <c r="T2" s="8" t="str">
         <f>C2</f>
         <v>Net wealth</v>
       </c>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9" t="s">
+      <c r="U2" s="8"/>
+      <c r="V2" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9" t="s">
+      <c r="W2" s="8"/>
+      <c r="X2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9" t="str">
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8" t="str">
         <f>G2</f>
         <v>Age</v>
       </c>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9" t="str">
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8" t="str">
         <f>H2</f>
         <v>Homeowner</v>
       </c>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="9" t="str">
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8" t="str">
         <f>I2</f>
         <v>Carowner</v>
       </c>
-      <c r="AE2" s="9"/>
-      <c r="AF2" s="9" t="str">
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8" t="str">
         <f>J2</f>
         <v>URE</v>
       </c>
-      <c r="AG2" s="9"/>
-      <c r="AH2" s="9" t="str">
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="8" t="str">
         <f>K2</f>
         <v>NNP</v>
       </c>
-      <c r="AI2" s="9"/>
-      <c r="AJ2" s="9" t="str">
+      <c r="AI2" s="8"/>
+      <c r="AJ2" s="8" t="str">
         <f>L2</f>
         <v>Liabilities</v>
       </c>
-      <c r="AK2" s="9"/>
+      <c r="AK2" s="8"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -4087,18 +5159,18 @@
       </c>
     </row>
     <row r="14" spans="1:37" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="T14" s="8" t="s">
+      <c r="T14" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="U14" s="8"/>
-      <c r="V14" s="8" t="s">
+      <c r="U14" s="9"/>
+      <c r="V14" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="W14" s="8"/>
-      <c r="X14" s="8" t="s">
+      <c r="W14" s="9"/>
+      <c r="X14" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="Y14" s="8"/>
+      <c r="Y14" s="9"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -4522,6 +5594,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
     <mergeCell ref="AD2:AE2"/>
     <mergeCell ref="AF2:AG2"/>
     <mergeCell ref="AH2:AI2"/>
@@ -4529,11 +5606,6 @@
     <mergeCell ref="T14:U14"/>
     <mergeCell ref="V14:W14"/>
     <mergeCell ref="X14:Y14"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
     <mergeCell ref="AB2:AC2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4541,12 +5613,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA56"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>